<commit_message>
Stand 02.01.2023, 22:50 Uhr
</commit_message>
<xml_diff>
--- a/Code Analysis/data-analysis/content-analysis/coding-matrix.xlsx
+++ b/Code Analysis/data-analysis/content-analysis/coding-matrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annesophie/Desktop/Visual_Communication_of_Climate_Change/Code Analysis/downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annesophie/Desktop/Visual_Communication_of_Climate_Change/Code Analysis/data-analysis/content-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA693367-DC16-C94C-82A8-A95239AB4399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F300254-7CBD-9541-8370-AAD99B9E80E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="30000" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>CU</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>SYNEC</t>
+  </si>
+  <si>
+    <t>IDPROM</t>
   </si>
 </sst>
 </file>
@@ -481,15 +484,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T1349"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,59 +503,62 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1000" xr:uid="{D97A428B-D241-0340-9177-F55AAC043707}">
       <formula1>1</formula1>
       <formula2>2000</formula2>
@@ -577,6 +583,10 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1349" xr:uid="{9CBAF5F8-DB38-C84F-92DC-170BEAA09FA6}">
       <formula1>"0,1,2,3,"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1683" xr:uid="{ACE101B5-07D3-C941-A98E-204D54406DE5}">
+      <formula1>0</formula1>
+      <formula2>26</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>